<commit_message>
Small refactoring was done.
</commit_message>
<xml_diff>
--- a/fixtures/excel/test-data.xlsx
+++ b/fixtures/excel/test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\test657\Desktop\del\playwright-custom-frame\playwright-custom-frame\fixtures\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2A1059-E2E8-439E-9B0C-5E9871F69FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F38A170-D729-498D-A94F-22D5D062AC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{AF9751E9-E2DF-458E-B6C8-88A94BEC73E0}"/>
   </bookViews>
@@ -151,7 +151,152 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0000FF"/>
+          <bgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4A86E8"/>
+          <bgColor rgb="FF4A86E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0000FF"/>
+          <bgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4A86E8"/>
+          <bgColor rgb="FF4A86E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0000FF"/>
+          <bgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4A86E8"/>
+          <bgColor rgb="FF4A86E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0000FF"/>
+          <bgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4A86E8"/>
+          <bgColor rgb="FF4A86E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -464,11 +609,12 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="28.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
   </cols>

</xml_diff>